<commit_message>
add assert check response birdview and infractions
</commit_message>
<xml_diff>
--- a/test_plan.xlsx
+++ b/test_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user1/Documents/learning/learn_iai_drive_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EBD78A-EFA5-E741-8F15-CC024BE63872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF8CA1B-F46E-9241-B2C7-B06972AD5B5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="580" windowWidth="27640" windowHeight="16040" xr2:uid="{573798C2-FE03-9345-9130-5C411E730E9A}"/>
   </bookViews>
@@ -700,7 +700,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:B55"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
add npc 25 cases, 26 will crash
</commit_message>
<xml_diff>
--- a/test_plan.xlsx
+++ b/test_plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user1/Documents/learning/learn_iai_drive_api/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF560C8F-3D20-C04C-ACC4-85E9853BA283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2DDBED-B3BA-CE4F-91DD-5C5E08516FA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1160" yWindow="580" windowWidth="27640" windowHeight="16040" xr2:uid="{573798C2-FE03-9345-9130-5C411E730E9A}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="137">
   <si>
     <t>case no.</t>
   </si>
@@ -438,6 +438,12 @@
   </si>
   <si>
     <t>Verify crash: 2 NPCs with random_seed big large 899999999999</t>
+  </si>
+  <si>
+    <t>TEST02001</t>
+  </si>
+  <si>
+    <t>Verify 25 NPCs</t>
   </si>
 </sst>
 </file>
@@ -789,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C64D70-901D-CD43-B001-059107A9FAF4}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+      <selection activeCell="B83" sqref="B83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1527,6 +1533,17 @@
         <v>133</v>
       </c>
     </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>135</v>
+      </c>
+      <c r="B78" t="s">
+        <v>136</v>
+      </c>
+      <c r="C78" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>